<commit_message>
Module 10 Challenge COMPLETED
</commit_message>
<xml_diff>
--- a/Images/Additional images.xlsx
+++ b/Images/Additional images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luispsalazar/Desktop/Mission-to-Mars/Images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD388E8E-3018-7C40-806E-52DADB6CF654}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BB2908-9F7B-4B42-99C0-FEFC543AB80E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47520" yWindow="240" windowWidth="28040" windowHeight="17440" xr2:uid="{BB071BCA-5F18-A842-B4FC-84AF881F7F55}"/>
+    <workbookView xWindow="-25440" yWindow="-4660" windowWidth="28040" windowHeight="25080" xr2:uid="{BB071BCA-5F18-A842-B4FC-84AF881F7F55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,6 +158,182 @@
             <a:schemeClr val="accent2"/>
           </a:solidFill>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>132882</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{868F46CE-2532-354F-92C6-A1479DCA464A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="977900" y="6108700"/>
+          <a:ext cx="7772400" cy="9060982"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rounded Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1C4C45C-A2BC-F448-9CE7-FEC70E8AA1BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="12725400"/>
+          <a:ext cx="7442200" cy="558800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>649048</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>81995</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>803511</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>31195</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Left Arrow 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37E1B326-7DD0-E94E-AEA3-AEE6A490D112}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20345773">
+          <a:off x="3951048" y="12070795"/>
+          <a:ext cx="1805463" cy="355600"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj2" fmla="val 49999"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -488,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AEC3A8-BB91-D04E-9EE9-159F2C01C6A4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>